<commit_message>
Added the correct string for doors within layout(excel file)
</commit_message>
<xml_diff>
--- a/BoardLayout.xlsx
+++ b/BoardLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\dev\eclipse_workspace\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGameITCM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="20">
   <si>
     <t>W</t>
   </si>
@@ -57,6 +57,33 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>WU</t>
+  </si>
+  <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>EL</t>
   </si>
 </sst>
 </file>
@@ -594,7 +621,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA16" sqref="AA16"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +705,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>4</v>
@@ -847,7 +874,7 @@
         <v>7</v>
       </c>
       <c r="N4" s="27" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>7</v>
@@ -894,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>9</v>
@@ -1066,7 +1093,7 @@
         <v>1</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="T7" s="5" t="s">
         <v>2</v>
@@ -1086,7 +1113,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>1</v>
@@ -1335,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>8</v>
@@ -1731,7 +1758,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>0</v>
@@ -1769,7 +1796,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>5</v>
@@ -1950,7 +1977,7 @@
         <v>1</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="T20" s="5" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Created failing test for targets and adjcs
</commit_message>
<xml_diff>
--- a/BoardLayout.xlsx
+++ b/BoardLayout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="30">
   <si>
     <t>W</t>
   </si>
@@ -87,6 +87,33 @@
   </si>
   <si>
     <t>WL</t>
+  </si>
+  <si>
+    <t>White =   Locations with only walkways as adjacent locations</t>
+  </si>
+  <si>
+    <t>Brown = Locations that are at each edge of the board</t>
+  </si>
+  <si>
+    <t>Purple = Locations that are beside a room cell that is not a doorway</t>
+  </si>
+  <si>
+    <t>Yellow = Locations that are adjacent to a doorway with needed direction (i.e., the adjacency list will include the doorway). Test all four directions.</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>Dark Green = Locations that are doorways (should have only one adjacent cell)</t>
+  </si>
+  <si>
+    <t>Red = Walkway test targets</t>
+  </si>
+  <si>
+    <t>Navy = targets when leaving a room</t>
+  </si>
+  <si>
+    <t>Orange = targets when entering room</t>
   </si>
 </sst>
 </file>
@@ -102,7 +129,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +151,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -339,8 +414,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +735,7 @@
       <c r="E1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="37" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -681,7 +768,7 @@
       <c r="P1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -775,7 +862,7 @@
       <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="33" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="22" t="s">
@@ -917,10 +1004,10 @@
       <c r="D5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="41" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -944,7 +1031,7 @@
       <c r="M5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="22" t="s">
+      <c r="N5" s="34" t="s">
         <v>1</v>
       </c>
       <c r="O5" s="7" t="s">
@@ -973,7 +1060,7 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="42" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="22" t="s">
@@ -1118,7 +1205,7 @@
       <c r="C8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="33" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="22" t="s">
@@ -1154,7 +1241,7 @@
       <c r="O8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="P8" s="22" t="s">
+      <c r="P8" s="42" t="s">
         <v>1</v>
       </c>
       <c r="Q8" s="22" t="s">
@@ -1234,7 +1321,7 @@
       <c r="S9" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="T9" s="22" t="s">
+      <c r="T9" s="39" t="s">
         <v>1</v>
       </c>
       <c r="U9" s="24" t="s">
@@ -1364,7 +1451,7 @@
       <c r="Q11" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="44" t="s">
         <v>11</v>
       </c>
       <c r="S11" s="2" t="s">
@@ -1381,10 +1468,10 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="34" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="22" t="s">
@@ -1642,8 +1729,8 @@
       <c r="S15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="T15" s="27" t="s">
-        <v>8</v>
+      <c r="T15" s="45" t="s">
+        <v>25</v>
       </c>
       <c r="U15" s="9" t="s">
         <v>8</v>
@@ -1730,7 +1817,7 @@
       <c r="C17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="40" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="22" t="s">
@@ -1760,7 +1847,7 @@
       <c r="M17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="38" t="s">
         <v>13</v>
       </c>
       <c r="O17" s="3" t="s">
@@ -1834,7 +1921,7 @@
       <c r="O18" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P18" s="22" t="s">
+      <c r="P18" s="39" t="s">
         <v>1</v>
       </c>
       <c r="Q18" s="22" t="s">
@@ -1979,7 +2066,7 @@
       <c r="R20" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="S20" s="5" t="s">
+      <c r="S20" s="38" t="s">
         <v>12</v>
       </c>
       <c r="T20" s="5" t="s">
@@ -2076,7 +2163,7 @@
       <c r="E22" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="25" t="s">
+      <c r="F22" s="36" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="25" t="s">
@@ -2106,10 +2193,10 @@
       <c r="O22" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="P22" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="25" t="s">
+      <c r="P22" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="36" t="s">
         <v>1</v>
       </c>
       <c r="R22" s="7" t="s">
@@ -2191,6 +2278,46 @@
       </c>
       <c r="U23">
         <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>